<commit_message>
new run with new features
</commit_message>
<xml_diff>
--- a/features2prediction/weebit/classification_evaluation.xlsx
+++ b/features2prediction/weebit/classification_evaluation.xlsx
@@ -26,16 +26,28 @@
     <t>threshold_socre</t>
   </si>
   <si>
+    <t>SVC rbf</t>
+  </si>
+  <si>
+    <t>MLP-deep</t>
+  </si>
+  <si>
+    <t>MLP 128</t>
+  </si>
+  <si>
+    <t>MLP 16</t>
+  </si>
+  <si>
+    <t>LinearSVC</t>
+  </si>
+  <si>
+    <t>SVC poly</t>
+  </si>
+  <si>
     <t>GradientBoostingClassifier</t>
   </si>
   <si>
-    <t>MLP 128</t>
-  </si>
-  <si>
-    <t>SVC rbf</t>
-  </si>
-  <si>
-    <t>MLP-deep</t>
+    <t>LogisticRegressionCV</t>
   </si>
   <si>
     <t>MLP 32</t>
@@ -44,19 +56,7 @@
     <t>MLP 64</t>
   </si>
   <si>
-    <t>MLP 16</t>
-  </si>
-  <si>
-    <t>LogisticRegressionCV</t>
-  </si>
-  <si>
     <t>RandomForestClassifier</t>
-  </si>
-  <si>
-    <t>LinearSVC</t>
-  </si>
-  <si>
-    <t>SVC poly</t>
   </si>
   <si>
     <t>SVC sigmoid</t>
@@ -432,13 +432,13 @@
         <v>3</v>
       </c>
       <c r="B2" t="n">
-        <v>0.6827</v>
+        <v>0.717</v>
       </c>
       <c r="C2" t="n">
-        <v>0.6827</v>
+        <v>0.717</v>
       </c>
       <c r="D2" t="n">
-        <v>0.908</v>
+        <v>0.9272</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -446,13 +446,13 @@
         <v>4</v>
       </c>
       <c r="B3" t="n">
-        <v>0.6758</v>
+        <v>0.6813</v>
       </c>
       <c r="C3" t="n">
-        <v>0.6758</v>
+        <v>0.6813</v>
       </c>
       <c r="D3" t="n">
-        <v>0.908</v>
+        <v>0.9245</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -460,13 +460,13 @@
         <v>5</v>
       </c>
       <c r="B4" t="n">
-        <v>0.6854</v>
+        <v>0.6827</v>
       </c>
       <c r="C4" t="n">
-        <v>0.6854</v>
+        <v>0.6827</v>
       </c>
       <c r="D4" t="n">
-        <v>0.9066</v>
+        <v>0.9217</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -474,13 +474,13 @@
         <v>6</v>
       </c>
       <c r="B5" t="n">
-        <v>0.6621</v>
+        <v>0.6841</v>
       </c>
       <c r="C5" t="n">
-        <v>0.6621</v>
+        <v>0.6841</v>
       </c>
       <c r="D5" t="n">
-        <v>0.9052</v>
+        <v>0.9217</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -488,13 +488,13 @@
         <v>7</v>
       </c>
       <c r="B6" t="n">
-        <v>0.6676</v>
+        <v>0.6731</v>
       </c>
       <c r="C6" t="n">
-        <v>0.6676</v>
+        <v>0.6731</v>
       </c>
       <c r="D6" t="n">
-        <v>0.9011</v>
+        <v>0.919</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -502,13 +502,13 @@
         <v>8</v>
       </c>
       <c r="B7" t="n">
-        <v>0.6731</v>
+        <v>0.6772</v>
       </c>
       <c r="C7" t="n">
-        <v>0.6731</v>
+        <v>0.6772</v>
       </c>
       <c r="D7" t="n">
-        <v>0.8997000000000001</v>
+        <v>0.919</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -516,13 +516,13 @@
         <v>9</v>
       </c>
       <c r="B8" t="n">
-        <v>0.6621</v>
+        <v>0.7033</v>
       </c>
       <c r="C8" t="n">
-        <v>0.6621</v>
+        <v>0.7033</v>
       </c>
       <c r="D8" t="n">
-        <v>0.8956</v>
+        <v>0.9147999999999999</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -530,13 +530,13 @@
         <v>10</v>
       </c>
       <c r="B9" t="n">
-        <v>0.6552</v>
+        <v>0.6813</v>
       </c>
       <c r="C9" t="n">
-        <v>0.6552</v>
+        <v>0.6813</v>
       </c>
       <c r="D9" t="n">
-        <v>0.886</v>
+        <v>0.9147999999999999</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -544,13 +544,13 @@
         <v>11</v>
       </c>
       <c r="B10" t="n">
-        <v>0.6511</v>
+        <v>0.6813</v>
       </c>
       <c r="C10" t="n">
-        <v>0.6511</v>
+        <v>0.6813</v>
       </c>
       <c r="D10" t="n">
-        <v>0.8804999999999999</v>
+        <v>0.9121</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -558,13 +558,13 @@
         <v>12</v>
       </c>
       <c r="B11" t="n">
-        <v>0.6552</v>
+        <v>0.6786</v>
       </c>
       <c r="C11" t="n">
-        <v>0.6552</v>
+        <v>0.6786</v>
       </c>
       <c r="D11" t="n">
-        <v>0.8777</v>
+        <v>0.9121</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -572,13 +572,13 @@
         <v>13</v>
       </c>
       <c r="B12" t="n">
-        <v>0.6387</v>
+        <v>0.6772</v>
       </c>
       <c r="C12" t="n">
-        <v>0.6387</v>
+        <v>0.6772</v>
       </c>
       <c r="D12" t="n">
-        <v>0.8764</v>
+        <v>0.9107</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -586,13 +586,13 @@
         <v>14</v>
       </c>
       <c r="B13" t="n">
-        <v>0.5632</v>
+        <v>0.6016</v>
       </c>
       <c r="C13" t="n">
-        <v>0.5632</v>
+        <v>0.6016</v>
       </c>
       <c r="D13" t="n">
-        <v>0.8104</v>
+        <v>0.8502999999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>